<commit_message>
updated analysis and figures
</commit_message>
<xml_diff>
--- a/tables_figures/final-tables_figures/Tables_LakeErie.xlsx
+++ b/tables_figures/final-tables_figures/Tables_LakeErie.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trentu-my.sharepoint.com/personal/sandraklemet_trentu_ca/Documents/Documents/Etudes/Trent/Xenopoulos lab/Projects/LakeErie_animal-excretion/tables_figures/final-tables_figures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sklem\OneDrive - Trent University\Documents\Etudes\Trent\Xenopoulos lab\Projects\LakeErie_animal-excretion\tables_figures\final-tables_figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="522" documentId="8_{0D343ED2-F8EF-47C9-B887-37799D7FBA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{661B8426-C886-4D0F-8F75-20632C825BD0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046A001F-BE88-4028-A1F8-A9829B7EE410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10660" activeTab="1" xr2:uid="{7E10462F-BD6C-49F1-8394-5EAC03425A95}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10600" activeTab="3" xr2:uid="{7E10462F-BD6C-49F1-8394-5EAC03425A95}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Table S8" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="112">
   <si>
     <t>n</t>
   </si>
@@ -220,9 +219,6 @@
     <t>response</t>
   </si>
   <si>
-    <t>region</t>
-  </si>
-  <si>
     <t>N load (tonnes/yr)</t>
   </si>
   <si>
@@ -262,166 +258,10 @@
     <t>∆AIC</t>
   </si>
   <si>
-    <r>
-      <t>Mass-specifc N excr  ~ δ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>15</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N + (1|Species)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Mass-specifc N excr  ~ δ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>13</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C  + (1|Species)</t>
-    </r>
-  </si>
-  <si>
     <t>Mass-specifc N excr  ~  (1|Species)</t>
   </si>
   <si>
-    <r>
-      <t>Mass-specifc P excr  ~ δ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>15</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N  + (1|Species)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Mass-specifc P excr  ~ δ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>13</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C  + (1|Species)</t>
-    </r>
-  </si>
-  <si>
     <t>Mass-specifc P excr  ~  (1|Species)</t>
-  </si>
-  <si>
-    <r>
-      <t>Mass-specifc N:P excr  ~ δ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>15</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>N  + (1|Species)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Mass-specifc N:P excr  ~ δ</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>13</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C  + (1|Species)</t>
-    </r>
   </si>
   <si>
     <t>Mass-specifc N:P excr  ~  (1|Species)</t>
@@ -487,25 +327,211 @@
     <t>Turnover time (h)</t>
   </si>
   <si>
-    <t>9496.65 ± 4099.34</t>
-  </si>
-  <si>
-    <t>1682.04 ± 726.07</t>
-  </si>
-  <si>
-    <t>290.84 ± 125.54</t>
-  </si>
-  <si>
-    <t>87.24 ± 37.66</t>
-  </si>
-  <si>
     <t>0.08 ± 0.13</t>
+  </si>
+  <si>
+    <t>Chemical form</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>SRP</t>
+  </si>
+  <si>
+    <t>TKN</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tributary </t>
+  </si>
+  <si>
+    <t>949.67 ± 409.93</t>
+  </si>
+  <si>
+    <t>168.2 ± 72.61</t>
+  </si>
+  <si>
+    <t>29.08 ± 12.55</t>
+  </si>
+  <si>
+    <t>8.72 ± 3.77</t>
+  </si>
+  <si>
+    <t>Tissue C:N (molar)</t>
+  </si>
+  <si>
+    <t>4.92 ± 0.11</t>
+  </si>
+  <si>
+    <t>3.33 ± 0.13</t>
+  </si>
+  <si>
+    <t>3.57 ± 0.28</t>
+  </si>
+  <si>
+    <t>Mass-specifc N excr  ~ C:N  + (1|Species)</t>
+  </si>
+  <si>
+    <t>Mass-specifc N excr  ~ N * Season + (1|Species)</t>
+  </si>
+  <si>
+    <r>
+      <t>Mass-specifc N excr  ~ δ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>N * Season + (1|Species)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mass-specifc N excr  ~ δ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>C  + (1|Species)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mass-specifc P excr  ~ δ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>N  + (1|Species)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mass-specifc P excr  ~ δ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>C  + (1|Species)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mass-specifc N:P excr  ~ δ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>N  + (1|Species)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mass-specifc N:P excr  ~ δ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>C  + (1|Species)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.000"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,9 +568,7 @@
       <family val="1"/>
     </font>
     <font>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -590,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -640,7 +664,6 @@
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -650,7 +673,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00EAFD5C-95BC-47EC-BF66-7189EEA6C490}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -980,7 +1025,9 @@
     <col min="6" max="6" width="9.90625" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.26953125" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7265625" style="9"/>
-    <col min="9" max="10" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -1071,7 +1118,7 @@
         <v>2.3126165199541102</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K26" si="0">J3/I3</f>
+        <f t="shared" ref="K3:K29" si="0">J3/I3</f>
         <v>0.73220274080990966</v>
       </c>
     </row>
@@ -1256,539 +1303,620 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="C10" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="13">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="6">
+        <v>3.1553742640000002</v>
+      </c>
+      <c r="G10" s="4">
+        <v>3.6383263170000002</v>
+      </c>
+      <c r="H10" s="6">
+        <v>4.0151993564831422E-2</v>
+      </c>
+      <c r="I10" s="10">
+        <v>3.3331799291666599</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0.13383381906632499</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>4.0151993564831422E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="D10" s="3">
-        <v>6</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="4">
-        <v>17.156048004157999</v>
-      </c>
-      <c r="G10" s="4">
-        <v>257.08077270788903</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0.8446738818699121</v>
-      </c>
-      <c r="I10" s="10">
-        <v>108.857118772098</v>
-      </c>
-      <c r="J10" s="10">
-        <v>91.948765082402105</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>0.8446738818699121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="D11" s="3">
         <v>6</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" s="4">
-        <v>3.2927501871101801</v>
+        <v>17.156048004157999</v>
       </c>
       <c r="G11" s="4">
-        <v>72.097783155650305</v>
+        <v>257.08077270788903</v>
       </c>
       <c r="H11" s="6">
-        <v>1.3628137102538971</v>
+        <v>0.8446738818699121</v>
       </c>
       <c r="I11" s="10">
-        <v>19.280703668212499</v>
+        <v>108.857118772098</v>
       </c>
       <c r="J11" s="10">
-        <v>26.276007302382599</v>
+        <v>91.948765082402105</v>
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>1.3628137102538971</v>
+        <v>0.8446738818699121</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C12" s="5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D12" s="3">
         <v>6</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="4">
-        <v>1.6103268234405399</v>
+        <v>3.2927501871101801</v>
       </c>
       <c r="G12" s="4">
-        <v>6.1507843836814198</v>
+        <v>72.097783155650305</v>
       </c>
       <c r="H12" s="6">
-        <v>0.53331537144886365</v>
+        <v>1.3628137102538971</v>
       </c>
       <c r="I12" s="10">
-        <v>3.3337677352144102</v>
+        <v>19.280703668212499</v>
       </c>
       <c r="J12" s="10">
-        <v>1.77794957803011</v>
+        <v>26.276007302382599</v>
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>0.53331537144886365</v>
+        <v>1.3628137102538971</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D13" s="3">
         <v>6</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="19">
-        <v>4.6899999999999997E-3</v>
-      </c>
-      <c r="G13" s="19">
-        <v>5.04E-2</v>
+      <c r="E13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1.6103268234405399</v>
+      </c>
+      <c r="G13" s="4">
+        <v>6.1507843836814198</v>
       </c>
       <c r="H13" s="6">
-        <v>0.93566649507428845</v>
+        <v>0.53331537144886365</v>
       </c>
       <c r="I13" s="10">
-        <v>2.0995079285714199E-2</v>
+        <v>3.3337677352144102</v>
       </c>
       <c r="J13" s="10">
-        <v>1.9644392249071E-2</v>
+        <v>1.77794957803011</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>0.93566649507428845</v>
+        <v>0.53331537144886365</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C14" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D14" s="3">
         <v>6</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F14" s="19">
-        <v>6.6874224030000002</v>
+        <v>4.6899999999999997E-3</v>
       </c>
       <c r="G14" s="19">
-        <v>9.5257914939999999</v>
+        <v>5.04E-2</v>
       </c>
       <c r="H14" s="6">
-        <v>0.16145851006903911</v>
+        <v>0.93566649507428845</v>
       </c>
       <c r="I14" s="10">
-        <v>8.1493068864999998</v>
+        <v>2.0995079285714199E-2</v>
       </c>
       <c r="J14" s="10">
-        <v>1.3157749479896499</v>
+        <v>1.9644392249071E-2</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>0.16145851006903911</v>
+        <v>0.93566649507428845</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C15" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" s="3">
         <v>6</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>25</v>
+      <c r="E15" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="F15" s="19">
-        <v>-25.891241690000001</v>
+        <v>6.6874224030000002</v>
       </c>
       <c r="G15" s="19">
-        <v>-23.65066719</v>
+        <v>9.5257914939999999</v>
       </c>
       <c r="H15" s="6">
-        <v>-3.9498419781143553E-2</v>
+        <v>0.16145851006903911</v>
       </c>
       <c r="I15" s="10">
-        <v>-24.796957509999999</v>
+        <v>8.1493068864999998</v>
       </c>
       <c r="J15" s="10">
-        <v>0.97944063702516004</v>
+        <v>1.3157749479896499</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>-3.9498419781143553E-2</v>
+        <v>0.16145851006903911</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="3">
         <v>6</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>26</v>
+      <c r="E16" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="F16" s="19">
-        <v>43.39079031</v>
+        <v>-25.891241690000001</v>
       </c>
       <c r="G16" s="19">
-        <v>47.416577259999997</v>
+        <v>-23.65066719</v>
       </c>
       <c r="H16" s="6">
-        <v>3.0201909095104857E-2</v>
+        <v>-3.9498419781143553E-2</v>
       </c>
       <c r="I16" s="10">
-        <v>45.801451104999998</v>
+        <v>-24.796957509999999</v>
       </c>
       <c r="J16" s="10">
-        <v>1.3832912626970999</v>
+        <v>0.97944063702516004</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>3.0201909095104857E-2</v>
+        <v>-3.9498419781143553E-2</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C17" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" s="3">
         <v>6</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>30</v>
+      <c r="E17" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="F17" s="19">
-        <v>10.2791689</v>
+        <v>43.39079031</v>
       </c>
       <c r="G17" s="19">
-        <v>11.155228490000001</v>
+        <v>47.416577259999997</v>
       </c>
       <c r="H17" s="6">
-        <v>2.7766480787994045E-2</v>
+        <v>3.0201909095104857E-2</v>
       </c>
       <c r="I17" s="10">
-        <v>10.8646716866666</v>
+        <v>45.801451104999998</v>
       </c>
       <c r="J17" s="10">
-        <v>0.30167369765569102</v>
+        <v>1.3832912626970999</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>2.7766480787994045E-2</v>
+        <v>3.0201909095104857E-2</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C18" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D18" s="3">
         <v>6</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="19">
+        <v>10.2791689</v>
+      </c>
+      <c r="G18" s="19">
+        <v>11.155228490000001</v>
+      </c>
+      <c r="H18" s="6">
+        <v>2.7766480787994045E-2</v>
+      </c>
+      <c r="I18" s="10">
+        <v>10.8646716866666</v>
+      </c>
+      <c r="J18" s="10">
+        <v>0.30167369765569102</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>2.7766480787994045E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="3">
+        <v>6</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F19" s="19">
         <v>1.098260748</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G19" s="19">
         <v>1.4162833269999999</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H19" s="6">
         <v>9.8735667071949806E-2</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I19" s="10">
         <v>1.2784571734999901</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J19" s="10">
         <v>0.12622932184844099</v>
       </c>
-      <c r="K18">
+      <c r="K19">
         <f t="shared" si="0"/>
         <v>9.8735667071949806E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
+    <row r="20" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="3">
+        <v>6</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="19">
+        <v>4.7499695390000003</v>
+      </c>
+      <c r="G20" s="19">
+        <v>5.0604236770000002</v>
+      </c>
+      <c r="H20" s="19">
+        <v>2.2332734953806142E-2</v>
+      </c>
+      <c r="I20" s="10">
+        <v>4.9192410378333298</v>
+      </c>
+      <c r="J20" s="10">
+        <v>0.109860106271818</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="0"/>
+        <v>2.2332734953806142E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B21" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="D19" s="13">
-        <v>102</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="19">
-        <v>3.3479632499999998</v>
-      </c>
-      <c r="G19" s="19">
-        <v>40.737754649999999</v>
-      </c>
-      <c r="H19" s="6">
-        <v>0.53641309855540953</v>
-      </c>
-      <c r="I19" s="10">
-        <v>12.1661420900188</v>
-      </c>
-      <c r="J19" s="10">
-        <v>6.5260779759723704</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>0.53641309855540953</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="13">
-        <v>102</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="19">
-        <v>0.20891138715728699</v>
-      </c>
-      <c r="G20" s="19">
-        <v>18.627624300000001</v>
-      </c>
-      <c r="H20" s="6">
-        <v>1.3026258318854445</v>
-      </c>
-      <c r="I20" s="10">
-        <v>3.2210867729442998</v>
-      </c>
-      <c r="J20" s="10">
-        <v>4.1958708371817703</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="0"/>
-        <v>1.3026258318854445</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="D21" s="13">
         <v>102</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F21" s="19">
-        <v>0.43780606729883498</v>
+        <v>3.3479632499999998</v>
       </c>
       <c r="G21" s="19">
-        <v>18.593047258004599</v>
+        <v>40.737754649999999</v>
       </c>
       <c r="H21" s="6">
-        <v>0.93479773691793699</v>
+        <v>0.53641309855540953</v>
       </c>
       <c r="I21" s="10">
-        <v>5.1023960287145496</v>
+        <v>12.1661420900188</v>
       </c>
       <c r="J21" s="10">
-        <v>4.7697082605014298</v>
+        <v>6.5260779759723704</v>
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>0.93479773691793699</v>
+        <v>0.53641309855540953</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C22" s="5" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D22" s="13">
         <v>102</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>45</v>
+      <c r="E22" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="F22" s="19">
-        <v>1</v>
+        <v>0.20891138715728699</v>
       </c>
       <c r="G22" s="19">
-        <v>887</v>
+        <v>18.627624300000001</v>
       </c>
       <c r="H22" s="6">
-        <v>1.3841147434379779</v>
+        <v>1.3026258318854445</v>
       </c>
       <c r="I22" s="10">
-        <v>150.843137254901</v>
+        <v>3.2210867729442998</v>
       </c>
       <c r="J22" s="10">
-        <v>208.78421022094699</v>
+        <v>4.1958708371817703</v>
       </c>
       <c r="K22">
         <f t="shared" si="0"/>
-        <v>1.3841147434379779</v>
+        <v>1.3026258318854445</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C23" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D23" s="13">
-        <v>55</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>28</v>
+        <v>102</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="F23" s="19">
-        <v>5.0072538150000003</v>
+        <v>0.43780606729883498</v>
       </c>
       <c r="G23" s="19">
-        <v>13.59</v>
+        <v>18.593047258004599</v>
       </c>
       <c r="H23" s="6">
-        <v>0.17621448508944335</v>
+        <v>0.93479773691793699</v>
       </c>
       <c r="I23" s="10">
-        <v>9.2261850927999998</v>
-      </c>
-      <c r="J23" s="10" t="s">
-        <v>31</v>
+        <v>5.1023960287145496</v>
+      </c>
+      <c r="J23" s="10">
+        <v>4.7697082605014298</v>
       </c>
       <c r="K23">
         <f t="shared" si="0"/>
-        <v>0.17621448508944335</v>
+        <v>0.93479773691793699</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C24" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D24" s="13">
-        <v>55</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>29</v>
+        <v>102</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F24" s="19">
-        <v>-26.521341150000001</v>
+        <v>1</v>
       </c>
       <c r="G24" s="19">
-        <v>-13.5</v>
+        <v>887</v>
       </c>
       <c r="H24" s="6">
-        <v>-0.13713131337330131</v>
+        <v>1.3841147434379779</v>
       </c>
       <c r="I24" s="10">
-        <v>-19.134563428545398</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>32</v>
+        <v>150.843137254901</v>
+      </c>
+      <c r="J24" s="10">
+        <v>208.78421022094699</v>
       </c>
       <c r="K24">
         <f t="shared" si="0"/>
-        <v>-0.13713131337330131</v>
+        <v>1.3841147434379779</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D25" s="13">
         <v>55</v>
       </c>
       <c r="E25" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="19">
+        <v>5.0072538150000003</v>
+      </c>
+      <c r="G25" s="19">
+        <v>13.59</v>
+      </c>
+      <c r="H25" s="6">
+        <v>0.17621448508944335</v>
+      </c>
+      <c r="I25" s="10">
+        <v>9.2261850927999998</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="0"/>
+        <v>0.17621448508944335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="13">
+        <v>55</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="19">
+        <v>-26.521341150000001</v>
+      </c>
+      <c r="G26" s="19">
+        <v>-13.5</v>
+      </c>
+      <c r="H26" s="6">
+        <v>-0.13713131337330131</v>
+      </c>
+      <c r="I26" s="10">
+        <v>-19.134563428545398</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="0"/>
+        <v>-0.13713131337330131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="13">
+        <v>55</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F27" s="19">
         <v>38.528017779999999</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G27" s="19">
         <v>52.43</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H27" s="6">
         <v>6.5573100201909276E-2</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I27" s="10">
         <v>45.962858123090903</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J27" s="10">
         <v>3.0139271012715798</v>
       </c>
-      <c r="K25">
+      <c r="K27">
         <f t="shared" si="0"/>
         <v>6.5573100201909276E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="7" t="s">
+    <row r="28" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D28" s="31">
         <v>55</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E28" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F28" s="33">
         <v>10.66434507</v>
       </c>
-      <c r="G26" s="20">
+      <c r="G28" s="33">
         <v>16.329999999999998</v>
       </c>
-      <c r="H26" s="18">
+      <c r="H28" s="32">
         <v>8.440206336813974E-2</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I28" s="10">
         <v>12.919240196000001</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J28" s="10">
         <v>1.09041052969101</v>
       </c>
-      <c r="K26">
-        <f t="shared" si="0"/>
+      <c r="K28">
+        <f>J28/I28</f>
         <v>8.440206336813974E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="8" t="s">
+    <row r="29" spans="1:11" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="15">
+        <v>55</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" s="20">
+        <v>3.21</v>
+      </c>
+      <c r="G29" s="20">
+        <v>4.6851086640000004</v>
+      </c>
+      <c r="H29" s="20">
+        <v>7.9429008703033405E-2</v>
+      </c>
+      <c r="I29" s="10">
+        <v>3.5726964022908998</v>
+      </c>
+      <c r="J29" s="10">
+        <v>0.28377573363086001</v>
+      </c>
+      <c r="K29">
+        <f>J29/I29</f>
+        <v>7.9429008703033405E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C31" s="5"/>
@@ -1796,7 +1924,17 @@
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C32" s="5"/>
     </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C35" s="5"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1805,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CD3C6F-D001-4806-B08E-514F56FFD6B0}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1846,7 +1984,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C2" s="9">
         <v>30</v>
@@ -1877,7 +2015,7 @@
     <row r="3" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
       <c r="B3" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C3" s="9">
         <v>30</v>
@@ -1945,7 +2083,7 @@
         <v>30</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E5" s="21">
         <v>2.15481499999999E-5</v>
@@ -1972,28 +2110,28 @@
         <v>51</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C6" s="9">
         <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E6" s="12">
-        <v>4913.6893902278698</v>
+        <v>491.368939022787</v>
       </c>
       <c r="F6" s="12">
-        <v>17764.877022440302</v>
+        <v>1776.4877022440301</v>
       </c>
       <c r="G6" s="12">
         <v>0.43166192963429245</v>
       </c>
-      <c r="H6" s="10">
-        <v>9496.6496846584705</v>
+      <c r="H6" s="29">
+        <v>949.66496846584698</v>
       </c>
       <c r="I6" s="10">
-        <v>4099.3421279405702</v>
+        <v>409.93421279405698</v>
       </c>
       <c r="J6" s="10">
         <f t="shared" si="0"/>
@@ -2003,32 +2141,32 @@
     <row r="7" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C7" s="9">
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E7" s="12">
-        <v>870.30954079326602</v>
+        <v>87.030954079326605</v>
       </c>
       <c r="F7" s="12">
-        <v>3146.5037237390102</v>
+        <v>314.65037237390101</v>
       </c>
       <c r="G7" s="12">
         <v>0.43166192963429351</v>
       </c>
-      <c r="H7" s="10">
-        <v>1682.0405544084099</v>
+      <c r="H7" s="29">
+        <v>168.20405544084099</v>
       </c>
       <c r="I7" s="10">
-        <v>726.07287143907104</v>
+        <v>72.607287143907101</v>
       </c>
       <c r="J7" s="10">
         <f t="shared" si="0"/>
-        <v>0.43166192963429351</v>
+        <v>0.43166192963429345</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -2040,26 +2178,26 @@
         <v>8</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E8" s="12">
-        <v>150.482571418248</v>
+        <v>15.0482571418248</v>
       </c>
       <c r="F8" s="12">
-        <v>544.05237347365096</v>
+        <v>54.405237347365102</v>
       </c>
       <c r="G8" s="12">
         <v>0.4316619296342904</v>
       </c>
-      <c r="H8" s="10">
-        <v>290.83650815368799</v>
+      <c r="H8" s="29">
+        <v>29.083650815368799</v>
       </c>
       <c r="I8" s="10">
-        <v>125.54304831771999</v>
+        <v>12.554304831772001</v>
       </c>
       <c r="J8" s="10">
         <f t="shared" si="0"/>
-        <v>0.4316619296342904</v>
+        <v>0.43166192963429045</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
@@ -2070,27 +2208,27 @@
       <c r="C9" s="14">
         <v>8</v>
       </c>
-      <c r="D9" s="24" t="s">
-        <v>98</v>
+      <c r="D9" s="23" t="s">
+        <v>99</v>
       </c>
       <c r="E9" s="16">
-        <v>45.138888899999998</v>
+        <v>4.5138888899999996</v>
       </c>
       <c r="F9" s="16">
-        <v>163.19444444999999</v>
+        <v>16.319444444999998</v>
       </c>
       <c r="G9" s="16">
         <v>0.43166192963429162</v>
       </c>
-      <c r="H9" s="10">
-        <v>87.239583334374998</v>
+      <c r="H9" s="29">
+        <v>8.7239583334374995</v>
       </c>
       <c r="I9" s="10">
-        <v>37.6580068826079</v>
+        <v>3.7658006882607902</v>
       </c>
       <c r="J9" s="10">
         <f t="shared" si="0"/>
-        <v>0.43166192963429162</v>
+        <v>0.43166192963429167</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
@@ -2145,15 +2283,15 @@
         <v>57</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B2" s="12">
         <f>H2/E2</f>
@@ -2164,7 +2302,7 @@
         <v>39.666451499631584</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="H2">
         <v>413.26921119487099</v>
@@ -2175,7 +2313,7 @@
     </row>
     <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B3" s="12">
         <f>I2/E3</f>
@@ -2186,13 +2324,13 @@
         <v>5.778795109503295</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B4" s="12">
         <f>H2/E4</f>
@@ -2203,12 +2341,12 @@
         <v>0.81335544109016056</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B5" s="16">
         <f>I2/E5</f>
@@ -2219,7 +2357,7 @@
         <v>0.44588663812313706</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F5" s="10"/>
     </row>
@@ -2230,10 +2368,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57374BE3-3D12-4D5E-AD85-8268CE3AECB4}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2242,150 +2380,180 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="26" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="9">
+        <v>4</v>
+      </c>
+      <c r="C2" s="9">
+        <v>36</v>
+      </c>
+      <c r="D2" s="9">
+        <f>C2-MIN($C$2:$C$6)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="9">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9">
+        <v>36</v>
+      </c>
+      <c r="D3" s="9">
+        <f t="shared" ref="D3:D5" si="0">C3-MIN($C$2:$C$6)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="9">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9">
+        <v>35</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="9">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9">
+        <v>28</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B6" s="9">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9">
+        <v>28</v>
+      </c>
+      <c r="D6" s="9">
+        <f>C6-MIN($C$2:$C$6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="9">
+        <v>4</v>
+      </c>
+      <c r="C7" s="9">
+        <v>81</v>
+      </c>
+      <c r="D7" s="9">
+        <f>C7-MIN($C$7:$C$9)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="9">
+        <v>4</v>
+      </c>
+      <c r="C8" s="9">
+        <v>81</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" ref="D8:D9" si="1">C8-MIN($C$7:$C$9)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>36</v>
-      </c>
-      <c r="D2">
-        <f>C2-MIN($C$2:$C$4)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B9" s="9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9">
         <v>74</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>36</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D4" si="0">C3-MIN($C$2:$C$4)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>28</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>81</v>
-      </c>
-      <c r="D5">
-        <f>C5-MIN($C$5:$C$7)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>81</v>
-      </c>
-      <c r="D6">
-        <f t="shared" ref="D6:D7" si="1">C6-MIN($C$5:$C$7)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>74</v>
-      </c>
-      <c r="D7">
+      <c r="D9" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8">
+    <row r="10" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="9">
         <v>4</v>
       </c>
-      <c r="C8">
+      <c r="C10" s="9">
         <v>67</v>
       </c>
-      <c r="D8">
-        <f>C8-MIN($C$8:$C$10)</f>
+      <c r="D10" s="9">
+        <f>C10-MIN($C$10:$C$12)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9">
+    <row r="11" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="9">
         <v>4</v>
       </c>
-      <c r="C9">
+      <c r="C11" s="9">
         <v>81</v>
       </c>
-      <c r="D9">
-        <f t="shared" ref="D9:D10" si="2">C9-MIN($C$8:$C$10)</f>
+      <c r="D11" s="9">
+        <f t="shared" ref="D11:D12" si="2">C11-MIN($C$10:$C$12)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="27">
+    <row r="12" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="14">
         <v>3</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C12" s="14">
         <v>60</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D12" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2397,199 +2565,231 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EB70EB-667B-40AE-9B29-064778A65493}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" customWidth="1"/>
+    <col min="5" max="5" width="11.08984375" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="17" t="s">
+    </row>
+    <row r="2" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="13">
+        <v>13544</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="13">
+        <v>4470</v>
+      </c>
+      <c r="P3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3">
+        <v>413.26921119487099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="13">
+        <v>12591</v>
+      </c>
+      <c r="P4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4">
+        <v>13.429482113076901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="13">
+        <v>3381</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="13">
+        <v>41900</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="13">
+        <v>3440</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="13">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="13">
+        <v>3099</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="13">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="9">
-        <v>13544</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="9">
-        <v>4470</v>
-      </c>
-      <c r="O3" t="s">
-        <v>55</v>
-      </c>
-      <c r="P3">
-        <v>413.26921119487099</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="9">
-        <v>12591</v>
-      </c>
-      <c r="O4" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4">
-        <v>13.429482113076901</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="9">
-        <v>3381</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="D11" s="19">
+        <v>1147.6570311615701</v>
+      </c>
+      <c r="E11" s="19">
+        <v>238.24310028683499</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="9">
-        <v>3440</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="9">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="9">
-        <v>3099</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="9">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="D12" s="26">
+        <v>12439.757279077599</v>
+      </c>
+      <c r="E12" s="26">
+        <v>2951.7960619758001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="12">
-        <v>1149.5804537105801</v>
-      </c>
-      <c r="D10" s="12">
-        <v>238.64238521150801</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9" t="s">
+      <c r="D13" s="27">
+        <v>191142.316905477</v>
+      </c>
+      <c r="E13" s="27">
+        <v>33855.005646673999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="22">
-        <v>19470.265656047199</v>
-      </c>
-      <c r="D11" s="22">
-        <v>4620.0462114968404</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="12">
-        <v>1914626.6299531299</v>
-      </c>
-      <c r="D12" s="12">
-        <v>339117.45142437599</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="23">
-        <v>294035.59365066898</v>
-      </c>
-      <c r="D13" s="23">
-        <v>52079.397406746197</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C14" s="5"/>
+      <c r="D14" s="28">
+        <v>187862.429873307</v>
+      </c>
+      <c r="E14" s="28">
+        <v>33274.074140808298</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="D15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>